<commit_message>
Data Analysis and replace audio
</commit_message>
<xml_diff>
--- a/aoiConditions/test1Conditions.xlsx
+++ b/aoiConditions/test1Conditions.xlsx
@@ -599,12 +599,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>trainingaudio/16_kotapi2.wav</t>
+          <t>trainingaudio/16_kokapi2.wav</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>trainingaudio/16_kotapi1.wav</t>
+          <t>trainingaudio/16_kokapi1.wav</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1079,12 +1079,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>trainingaudio/16_kotapi2.wav</t>
+          <t>trainingaudio/16_kokapi2.wav</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>trainingaudio/16_kotapi1.wav</t>
+          <t>trainingaudio/16_kokapi1.wav</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">

</xml_diff>